<commit_message>
updated spreadsheets for ACM mortality
</commit_message>
<xml_diff>
--- a/debate/ACM/UCOD_by_age_year_analysis.xlsx
+++ b/debate/ACM/UCOD_by_age_year_analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\debate\acm_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\covid\debate\ACM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7E84D051-6B02-4C98-B39E-5DC59B7A2161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE03A528-D365-46F7-B45C-A47DE8F950FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9AA18A5B-79EA-4532-B807-4FDA8DB02634}"/>
   </bookViews>
@@ -19,15 +19,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">UCOD_by_age_year!$A$1:$G$161</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="53">
   <si>
     <t>Five-Year Age Groups</t>
   </si>
@@ -183,6 +196,9 @@
   </si>
   <si>
     <t>Column Labels</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -681,14 +697,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -6683,7 +6698,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5E240FDF-61BF-4C96-9B5B-62D5BDAC93BD}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5E240FDF-61BF-4C96-9B5B-62D5BDAC93BD}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:G23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -7247,10 +7262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E4BBDB-B47F-45A1-97BE-1C6EAF4754CC}">
-  <dimension ref="A3:G45"/>
+  <dimension ref="A3:Y45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:C27"/>
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7261,7 +7276,7 @@
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>50</v>
       </c>
@@ -7269,7 +7284,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>48</v>
       </c>
@@ -7292,279 +7307,282 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>3120</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5">
         <v>3164</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5">
         <v>3413</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>3569</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5">
         <v>3672</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5">
         <v>3503</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>10380</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>10258</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>12278</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6">
         <v>13407</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6">
         <v>12745</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6">
         <v>12777</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>19774</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>19513</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>23538</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
         <v>24900</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7">
         <v>22487</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7">
         <v>20934</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8">
         <v>27461</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8">
         <v>26969</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8">
         <v>32696</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8">
         <v>35195</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8">
         <v>31295</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8">
         <v>27775</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>31383</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9">
         <v>32209</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9">
         <v>40790</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9">
         <v>47079</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9">
         <v>43074</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9">
         <v>39674</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>37617</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>38638</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10">
         <v>48081</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10">
         <v>56403</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10">
         <v>50472</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10">
         <v>46983</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11">
         <v>42763</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11">
         <v>44348</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11">
         <v>56409</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11">
         <v>68536</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11">
         <v>61133</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11">
         <v>58353</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Y11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12">
         <v>64873</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12">
         <v>63739</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12">
         <v>76431</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12">
         <v>86144</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12">
         <v>73143</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12">
         <v>67271</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13">
         <v>99964</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13">
         <v>96654</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13">
         <v>114711</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13">
         <v>129893</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13">
         <v>110141</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13">
         <v>99502</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14">
         <v>160963</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14">
         <v>158453</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14">
         <v>183228</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14">
         <v>197608</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14">
         <v>168323</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14">
         <v>148600</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15">
         <v>213873</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15">
         <v>216484</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15">
         <v>257321</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15">
         <v>280563</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15">
         <v>249218</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15">
         <v>227934</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16">
         <v>251246</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16">
         <v>254412</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16">
         <v>306388</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16">
         <v>330984</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16">
         <v>306165</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16">
         <v>288996</v>
       </c>
     </row>
@@ -7572,22 +7590,22 @@
       <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17">
         <v>292532</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17">
         <v>301147</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17">
         <v>368119</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17">
         <v>393282</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17">
         <v>362416</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17">
         <v>338684</v>
       </c>
     </row>
@@ -7595,22 +7613,22 @@
       <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18">
         <v>321745</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18">
         <v>329493</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18">
         <v>398191</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18">
         <v>408867</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18">
         <v>407592</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18">
         <v>389791</v>
       </c>
     </row>
@@ -7618,22 +7636,22 @@
       <c r="A19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19">
         <v>353460</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19">
         <v>358534</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19">
         <v>423893</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19">
         <v>420786</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19">
         <v>417311</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19">
         <v>408397</v>
       </c>
     </row>
@@ -7641,22 +7659,22 @@
       <c r="A20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20">
         <v>385116</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20">
         <v>378916</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20">
         <v>439251</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20">
         <v>414900</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20">
         <v>408434</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20">
         <v>389919</v>
       </c>
     </row>
@@ -7664,22 +7682,22 @@
       <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21">
         <v>320069</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21">
         <v>317483</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21">
         <v>365686</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21">
         <v>336925</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21">
         <v>332016</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21">
         <v>312034</v>
       </c>
     </row>
@@ -7687,22 +7705,22 @@
       <c r="A22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22">
         <v>144846</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22">
         <v>146616</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22">
         <v>171236</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22">
         <v>155459</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22">
         <v>157396</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22">
         <v>149364</v>
       </c>
     </row>
@@ -7710,22 +7728,22 @@
       <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23">
         <v>2781185</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23">
         <v>2797030</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23">
         <v>3321660</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23">
         <v>3404500</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23">
         <v>3217033</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23">
         <v>3030491</v>
       </c>
     </row>
@@ -7733,10 +7751,10 @@
       <c r="A27" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="4">
         <v>2018</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <v>2019</v>
       </c>
       <c r="D27">

</xml_diff>